<commit_message>
BEXIS2/Core#1419 refactor excel template, remove makro template
</commit_message>
<xml_diff>
--- a/Modules/RPM/Template/BExISppTemplate_Clean.xlsx
+++ b/Modules/RPM/Template/BExISppTemplate_Clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\Bexis2\BEXIS2 - Core - Workspace\Core\Console\Workspace\Modules\RPM\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C705CA0-C1FD-4CC9-93D8-F5295BF6FD1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80958B-BBDD-4AEC-AFB6-76BC029BB3BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="8772" xr2:uid="{8A53DF21-A7E6-4853-9BDE-9FA1A4CF4B86}"/>
   </bookViews>
@@ -24,22 +24,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,10 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -394,16 +381,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
update excel template, add description row
</commit_message>
<xml_diff>
--- a/Modules/RPM/Template/BExISppTemplate_Clean.xlsx
+++ b/Modules/RPM/Template/BExISppTemplate_Clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\Bexis2\BEXIS2 - Core - Workspace\Core\Console\Workspace\Modules\RPM\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Schöne\source\repos\BEXIS2\BEXIS2-RC\Core\Console\Workspace\Modules\RPM\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80958B-BBDD-4AEC-AFB6-76BC029BB3BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1F58E4-A751-458D-B83C-EF511AA49C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="8772" xr2:uid="{8A53DF21-A7E6-4853-9BDE-9FA1A4CF4B86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8A53DF21-A7E6-4853-9BDE-9FA1A4CF4B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -81,9 +80,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -121,7 +120,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -227,7 +226,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -369,7 +368,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -380,17 +379,17 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
add rows to excel template for desctipion and missing values
</commit_message>
<xml_diff>
--- a/Modules/RPM/Template/BExISppTemplate_Clean.xlsx
+++ b/Modules/RPM/Template/BExISppTemplate_Clean.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\Bexis2\BEXIS2 - Core - Workspace\Core\Console\Workspace\Modules\RPM\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Schöne\source\repos\BEXIS2\BEXIS2-RC\Core\Console\Workspace\Modules\RPM\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80958B-BBDD-4AEC-AFB6-76BC029BB3BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E4DEDE-F66B-495F-B575-9B87B3B47EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="8772" xr2:uid="{8A53DF21-A7E6-4853-9BDE-9FA1A4CF4B86}"/>
+    <workbookView xWindow="7410" yWindow="4755" windowWidth="38700" windowHeight="15345" xr2:uid="{8A53DF21-A7E6-4853-9BDE-9FA1A4CF4B86}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,9 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -81,9 +80,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -121,7 +120,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -227,7 +226,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -369,7 +368,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -377,20 +376,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8217C9DE-1220-4F20-9DC0-91D639DC5F30}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>